<commit_message>
Minor fix of styles in cache
</commit_message>
<xml_diff>
--- a/demo/files/demo-00-test.xlsx
+++ b/demo/files/demo-00-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\www-domains\dev.loc\fast-excel-reader\demo\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6C5FEA-98EE-40DE-A8D8-66FBB3C3E76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131B6609-F453-4E35-9849-ABA19A72AA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7158" yWindow="0" windowWidth="13080" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,10 +68,9 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -485,7 +484,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
improved date handling; more tests
</commit_message>
<xml_diff>
--- a/demo/files/demo-00-test.xlsx
+++ b/demo/files/demo-00-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\www-domains\dev.loc\fast-excel-reader\demo\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131B6609-F453-4E35-9849-ABA19A72AA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E850FE5-BBA2-4411-8B61-117A83482CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7158" yWindow="0" windowWidth="13080" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="63510" yWindow="4125" windowWidth="17280" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,21 +36,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>logo</t>
-  </si>
-  <si>
-    <t>Excel</t>
-  </si>
-  <si>
-    <t>Word</t>
+    <t>James Bond</t>
+  </si>
+  <si>
+    <t>Ellen Louise Ripley</t>
+  </si>
+  <si>
+    <t>Captain Jack Sparrow</t>
+  </si>
+  <si>
+    <t>31.01.1753</t>
+  </si>
+  <si>
+    <t>random_int</t>
+  </si>
+  <si>
+    <t>birthday</t>
   </si>
 </sst>
 </file>
@@ -68,9 +75,10 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,12 +101,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -111,111 +120,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F94741B-E73B-5BD3-B727-9340B7585B74}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1280160" y="182880"/>
-          <a:ext cx="350520" cy="350520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Рисунок 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86EB524E-BB44-82AE-A3AD-604E7A56DCDA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1280160" y="487680"/>
-          <a:ext cx="342900" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -481,44 +385,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="17.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.62890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="1">
+        <v>102128</v>
+      </c>
+      <c r="C3">
+        <v>982630</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="27.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>222</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="C4">
+        <v>7239</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix date before 1900-03-01
</commit_message>
<xml_diff>
--- a/demo/files/demo-00-test.xlsx
+++ b/demo/files/demo-00-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\www-domains\dev.loc\fast-excel-reader\demo\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E850FE5-BBA2-4411-8B61-117A83482CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54BBB30-7340-4FCB-BEB9-2471C4B66D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63510" yWindow="4125" windowWidth="17280" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="17280" windowHeight="8904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,10 +101,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,16 +386,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="17.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -410,35 +411,42 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45</v>
-      </c>
-      <c r="C2">
-        <v>4573</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="3">
+        <v>61</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>102128</v>
+        <v>45</v>
       </c>
       <c r="C3">
-        <v>982630</v>
+        <v>4573</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>102128</v>
+      </c>
+      <c r="C4">
+        <v>982630</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>7239</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new methods: reset() & readNextRow()
</commit_message>
<xml_diff>
--- a/demo/files/demo-00-test.xlsx
+++ b/demo/files/demo-00-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\www-domains\dev.loc\fast-excel-reader\demo\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703ECEEB-C9F0-4902-86EA-28D69BABF06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E415D2-0D67-45CC-9E78-37FDDECD0433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58515" yWindow="915" windowWidth="21600" windowHeight="12270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59370" yWindow="480" windowWidth="21495" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>birthday</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -385,58 +388,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>45</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>4573</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
         <v>102128</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>982630</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>7239</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: if the cell is in text format, then the value should not be converted to a number fix: check active sheet
</commit_message>
<xml_diff>
--- a/demo/files/demo-00-test.xlsx
+++ b/demo/files/demo-00-test.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\www-domains\dev.loc\fast-excel-reader\demo\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E415D2-0D67-45CC-9E78-37FDDECD0433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676D3E21-D277-4EED-9A75-98ACE5809526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59370" yWindow="480" windowWidth="21495" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -60,12 +62,63 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Fraction</t>
+  </si>
+  <si>
+    <t>Scientific</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>3.2.24</t>
+  </si>
+  <si>
+    <t>3.2.24.7</t>
+  </si>
+  <si>
+    <t>3.2.24.d</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>3.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="d/m/yy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,13 +157,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -390,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -459,4 +522,156 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA43052-54AC-4F06-B375-ADA82BA4FA0C}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="10.05078125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="10">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B25E165-DEDA-4396-90DC-A7DA8A718E6A}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.62890625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11">
+        <v>45325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="12">
+        <v>45325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>